<commit_message>
Random Forest working for 4 labels now to try 2 labels
</commit_message>
<xml_diff>
--- a/DataCleaning/outliers.xlsx
+++ b/DataCleaning/outliers.xlsx
@@ -14,7 +14,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="59">
+  <si>
+    <t>ORDEM</t>
+  </si>
+  <si>
+    <t>DATA</t>
+  </si>
   <si>
     <t>AMOSTRA</t>
   </si>
@@ -191,6 +197,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -243,11 +252,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,13 +552,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AH22"/>
+  <dimension ref="A1:AJ22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:36">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -648,2155 +658,2269 @@
       <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="AI1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:36">
       <c r="A2" s="1">
         <v>174</v>
       </c>
-      <c r="B2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" t="s">
-        <v>38</v>
+      <c r="B2">
+        <v>175</v>
+      </c>
+      <c r="C2" s="2">
+        <v>43235</v>
       </c>
       <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
         <v>40</v>
       </c>
-      <c r="E2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2">
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2">
         <v>11.19</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>31.95</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>34.12</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>22.74</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>58.8</v>
       </c>
-      <c r="K2">
+      <c r="M2">
         <v>98.90000000000001</v>
       </c>
-      <c r="L2">
+      <c r="N2">
         <v>45</v>
       </c>
-      <c r="M2">
+      <c r="O2">
         <v>0.51</v>
       </c>
-      <c r="N2">
+      <c r="P2">
         <v>70</v>
       </c>
-      <c r="O2">
+      <c r="Q2">
         <v>70</v>
       </c>
-      <c r="P2">
+      <c r="R2">
         <v>57.5</v>
       </c>
-      <c r="Q2">
+      <c r="S2">
         <v>201.2</v>
       </c>
-      <c r="R2">
+      <c r="T2">
         <v>151</v>
       </c>
-      <c r="S2">
+      <c r="U2">
         <v>93</v>
       </c>
-      <c r="T2">
+      <c r="V2">
         <v>89.2</v>
       </c>
-      <c r="U2">
+      <c r="W2">
         <v>114.3</v>
       </c>
-      <c r="V2">
+      <c r="X2">
         <v>3.4</v>
       </c>
-      <c r="W2">
+      <c r="Y2">
         <v>39.7</v>
       </c>
-      <c r="X2">
+      <c r="Z2">
         <v>95</v>
       </c>
-      <c r="Y2">
+      <c r="AA2">
         <v>77</v>
       </c>
-      <c r="Z2">
+      <c r="AB2">
         <v>50</v>
       </c>
-      <c r="AA2">
+      <c r="AC2">
         <v>41</v>
       </c>
-      <c r="AB2">
+      <c r="AD2">
         <v>41</v>
       </c>
-      <c r="AC2">
+      <c r="AE2">
         <v>9</v>
       </c>
-      <c r="AD2">
+      <c r="AF2">
         <v>9</v>
       </c>
-      <c r="AE2">
+      <c r="AG2">
         <v>41</v>
       </c>
-      <c r="AF2">
+      <c r="AH2">
         <v>68.85245901639344</v>
       </c>
-      <c r="AG2">
+      <c r="AI2">
         <v>32.78688524590164</v>
       </c>
     </row>
-    <row r="3" spans="1:34">
+    <row r="3" spans="1:36">
       <c r="A3" s="1">
         <v>57</v>
       </c>
       <c r="B3">
+        <v>58</v>
+      </c>
+      <c r="C3" s="2">
+        <v>42285</v>
+      </c>
+      <c r="D3">
         <v>244</v>
       </c>
-      <c r="C3">
+      <c r="E3">
         <v>40</v>
       </c>
-      <c r="D3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3">
+      <c r="F3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3">
         <v>7.76</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>27</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>29.47</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>35.77</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>84.40000000000001</v>
       </c>
-      <c r="K3">
+      <c r="M3">
         <v>60.8</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>0.14</v>
       </c>
-      <c r="M3">
+      <c r="O3">
         <v>0.014</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>45</v>
       </c>
-      <c r="O3">
+      <c r="Q3">
         <v>55</v>
       </c>
-      <c r="P3">
+      <c r="R3">
         <v>16</v>
       </c>
-      <c r="Q3">
+      <c r="S3">
         <v>74.8</v>
       </c>
-      <c r="R3">
+      <c r="T3">
         <v>0</v>
       </c>
-      <c r="S3">
+      <c r="U3">
         <v>98.5</v>
       </c>
-      <c r="T3">
+      <c r="V3">
         <v>62.8</v>
       </c>
-      <c r="U3">
+      <c r="W3">
         <v>207.1</v>
       </c>
-      <c r="V3">
+      <c r="X3">
         <v>8.800000000000001</v>
       </c>
-      <c r="W3">
+      <c r="Y3">
         <v>28.6</v>
       </c>
-      <c r="X3">
+      <c r="Z3">
         <v>65</v>
       </c>
-      <c r="Y3">
+      <c r="AA3">
         <v>33</v>
       </c>
-      <c r="Z3">
+      <c r="AB3">
         <v>38</v>
       </c>
-      <c r="AA3">
+      <c r="AC3">
         <v>18</v>
       </c>
-      <c r="AB3">
+      <c r="AD3">
         <v>36</v>
       </c>
-      <c r="AC3">
+      <c r="AE3">
         <v>2</v>
       </c>
-      <c r="AD3">
+      <c r="AF3">
         <v>8</v>
       </c>
-      <c r="AE3">
+      <c r="AG3">
         <v>54</v>
       </c>
-      <c r="AF3">
+      <c r="AH3">
         <v>77.77777777777779</v>
       </c>
-      <c r="AG3">
+      <c r="AI3">
         <v>18.05555555555555</v>
       </c>
-      <c r="AH3">
+      <c r="AJ3">
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:34">
+    <row r="4" spans="1:36">
       <c r="A4" s="1">
         <v>140</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
+        <v>141</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4">
+        <v>36.28</v>
+      </c>
+      <c r="I4">
+        <v>22.93</v>
+      </c>
+      <c r="J4">
+        <v>33.24</v>
+      </c>
+      <c r="K4">
+        <v>7.55</v>
+      </c>
+      <c r="L4">
+        <v>97.59999999999999</v>
+      </c>
+      <c r="M4">
+        <v>68.7</v>
+      </c>
+      <c r="N4">
+        <v>1.55</v>
+      </c>
+      <c r="O4">
+        <v>2.04</v>
+      </c>
+      <c r="P4">
+        <v>80</v>
+      </c>
+      <c r="Q4">
+        <v>80</v>
+      </c>
+      <c r="R4">
+        <v>70</v>
+      </c>
+      <c r="S4">
+        <v>504</v>
+      </c>
+      <c r="T4">
+        <v>414</v>
+      </c>
+      <c r="U4">
+        <v>109.9</v>
+      </c>
+      <c r="V4">
+        <v>95.2</v>
+      </c>
+      <c r="W4">
+        <v>181.1</v>
+      </c>
+      <c r="X4">
+        <v>7.2</v>
+      </c>
+      <c r="Y4">
+        <v>32.1</v>
+      </c>
+      <c r="Z4">
+        <v>85</v>
+      </c>
+      <c r="AA4">
+        <v>53</v>
+      </c>
+      <c r="AB4">
+        <v>54</v>
+      </c>
+      <c r="AC4">
+        <v>40</v>
+      </c>
+      <c r="AD4">
+        <v>48</v>
+      </c>
+      <c r="AE4">
+        <v>6</v>
+      </c>
+      <c r="AF4">
+        <v>12</v>
+      </c>
+      <c r="AG4">
         <v>34</v>
       </c>
-      <c r="C4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4">
-        <v>36.28</v>
-      </c>
-      <c r="G4">
-        <v>22.93</v>
-      </c>
-      <c r="H4">
-        <v>33.24</v>
-      </c>
-      <c r="I4">
-        <v>7.55</v>
-      </c>
-      <c r="J4">
-        <v>97.59999999999999</v>
-      </c>
-      <c r="K4">
-        <v>68.7</v>
-      </c>
-      <c r="L4">
-        <v>1.55</v>
-      </c>
-      <c r="M4">
-        <v>2.04</v>
-      </c>
-      <c r="N4">
-        <v>80</v>
-      </c>
-      <c r="O4">
-        <v>80</v>
-      </c>
-      <c r="P4">
-        <v>70</v>
-      </c>
-      <c r="Q4">
-        <v>504</v>
-      </c>
-      <c r="R4">
-        <v>414</v>
-      </c>
-      <c r="S4">
-        <v>109.9</v>
-      </c>
-      <c r="T4">
-        <v>95.2</v>
-      </c>
-      <c r="U4">
-        <v>181.1</v>
-      </c>
-      <c r="V4">
-        <v>7.2</v>
-      </c>
-      <c r="W4">
-        <v>32.1</v>
-      </c>
-      <c r="X4">
-        <v>85</v>
-      </c>
-      <c r="Y4">
-        <v>53</v>
-      </c>
-      <c r="Z4">
-        <v>54</v>
-      </c>
-      <c r="AA4">
-        <v>40</v>
-      </c>
-      <c r="AB4">
-        <v>48</v>
-      </c>
-      <c r="AC4">
-        <v>6</v>
-      </c>
-      <c r="AD4">
-        <v>12</v>
-      </c>
-      <c r="AE4">
-        <v>34</v>
-      </c>
-      <c r="AF4">
+      <c r="AH4">
         <v>84.50704225352112</v>
       </c>
-      <c r="AG4">
+      <c r="AI4">
         <v>35.2112676056338</v>
       </c>
-      <c r="AH4">
+      <c r="AJ4">
         <v>152.5</v>
       </c>
     </row>
-    <row r="5" spans="1:34">
+    <row r="5" spans="1:36">
       <c r="A5" s="1">
         <v>148</v>
       </c>
-      <c r="B5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" t="s">
-        <v>39</v>
+      <c r="B5">
+        <v>149</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5">
         <v>16.55</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>22.3</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>36.9</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>24.25</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>98.09999999999999</v>
       </c>
-      <c r="K5">
+      <c r="M5">
         <v>71.90000000000001</v>
       </c>
-      <c r="L5">
+      <c r="N5">
         <v>0.24</v>
       </c>
-      <c r="M5">
+      <c r="O5">
         <v>2.76</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <v>80</v>
       </c>
-      <c r="O5">
+      <c r="Q5">
         <v>80</v>
       </c>
-      <c r="P5">
+      <c r="R5">
         <v>33.5</v>
       </c>
-      <c r="Q5">
+      <c r="S5">
         <v>241</v>
       </c>
-      <c r="R5">
+      <c r="T5">
         <v>151</v>
       </c>
-      <c r="S5">
+      <c r="U5">
         <v>127.7</v>
       </c>
-      <c r="T5">
+      <c r="V5">
         <v>118.2</v>
       </c>
-      <c r="U5">
+      <c r="W5">
         <v>199.4</v>
       </c>
-      <c r="V5">
+      <c r="X5">
         <v>6.7</v>
       </c>
-      <c r="W5">
+      <c r="Y5">
         <v>38.7</v>
       </c>
-      <c r="X5">
+      <c r="Z5">
         <v>91</v>
       </c>
-      <c r="Y5">
+      <c r="AA5">
         <v>60</v>
       </c>
-      <c r="Z5">
+      <c r="AB5">
         <v>63</v>
       </c>
-      <c r="AA5">
+      <c r="AC5">
         <v>59</v>
       </c>
-      <c r="AB5">
+      <c r="AD5">
         <v>61</v>
       </c>
-      <c r="AC5">
+      <c r="AE5">
         <v>2</v>
       </c>
-      <c r="AD5">
+      <c r="AF5">
         <v>11</v>
       </c>
-      <c r="AE5">
+      <c r="AG5">
         <v>26</v>
       </c>
-      <c r="AF5">
+      <c r="AH5">
         <v>63.01369863013699</v>
       </c>
-      <c r="AG5">
+      <c r="AI5">
         <v>5.47945205479452</v>
       </c>
     </row>
-    <row r="6" spans="1:34">
+    <row r="6" spans="1:36">
       <c r="A6" s="1">
         <v>156</v>
       </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
+      <c r="B6">
+        <v>157</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6">
+        <v>41</v>
+      </c>
+      <c r="F6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6">
         <v>19.85</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>21.54</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <v>33.71</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>24.91</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>85</v>
       </c>
-      <c r="K6">
+      <c r="M6">
         <v>49.9</v>
       </c>
-      <c r="L6">
+      <c r="N6">
         <v>1.27</v>
       </c>
-      <c r="M6">
+      <c r="O6">
         <v>2.48</v>
       </c>
-      <c r="N6">
+      <c r="P6">
         <v>60</v>
       </c>
-      <c r="O6">
+      <c r="Q6">
         <v>75</v>
       </c>
-      <c r="P6">
+      <c r="R6">
         <v>28.5</v>
       </c>
-      <c r="Q6">
+      <c r="S6">
         <v>192</v>
-      </c>
-      <c r="R6">
-        <v>102</v>
-      </c>
-      <c r="S6">
-        <v>111</v>
       </c>
       <c r="T6">
         <v>102</v>
       </c>
       <c r="U6">
+        <v>111</v>
+      </c>
+      <c r="V6">
+        <v>102</v>
+      </c>
+      <c r="W6">
         <v>177.1</v>
       </c>
-      <c r="V6">
+      <c r="X6">
         <v>6.4</v>
       </c>
-      <c r="W6">
+      <c r="Y6">
         <v>37.1</v>
       </c>
-      <c r="X6">
+      <c r="Z6">
         <v>90</v>
       </c>
-      <c r="Y6">
+      <c r="AA6">
         <v>59</v>
       </c>
-      <c r="Z6">
+      <c r="AB6">
         <v>46</v>
       </c>
-      <c r="AA6">
+      <c r="AC6">
         <v>40</v>
       </c>
-      <c r="AB6">
+      <c r="AD6">
         <v>43</v>
       </c>
-      <c r="AC6">
+      <c r="AE6">
         <v>3</v>
       </c>
-      <c r="AD6">
+      <c r="AF6">
         <v>11</v>
       </c>
-      <c r="AE6">
+      <c r="AG6">
         <v>43</v>
       </c>
-      <c r="AF6">
+      <c r="AH6">
         <v>58.57142857142858</v>
       </c>
-      <c r="AG6">
+      <c r="AI6">
         <v>11.26760563380282</v>
       </c>
-      <c r="AH6">
+      <c r="AJ6">
         <v>141.6666666666667</v>
       </c>
     </row>
-    <row r="7" spans="1:34">
+    <row r="7" spans="1:36">
       <c r="A7" s="1">
         <v>214</v>
       </c>
       <c r="B7">
+        <v>215</v>
+      </c>
+      <c r="C7" s="2">
+        <v>42285</v>
+      </c>
+      <c r="D7">
         <v>244</v>
       </c>
-      <c r="C7">
+      <c r="E7">
         <v>40</v>
       </c>
-      <c r="D7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7">
+      <c r="F7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7">
         <v>7.76</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>27</v>
       </c>
-      <c r="H7">
+      <c r="J7">
         <v>29.47</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <v>35.77</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <v>84.40000000000001</v>
       </c>
-      <c r="K7">
+      <c r="M7">
         <v>60.8</v>
       </c>
-      <c r="L7">
+      <c r="N7">
         <v>0.14</v>
       </c>
-      <c r="M7">
+      <c r="O7">
         <v>0.014</v>
       </c>
-      <c r="N7">
+      <c r="P7">
         <v>45</v>
       </c>
-      <c r="O7">
+      <c r="Q7">
         <v>55</v>
       </c>
-      <c r="P7">
+      <c r="R7">
         <v>16</v>
       </c>
-      <c r="Q7">
+      <c r="S7">
         <v>74.8</v>
       </c>
-      <c r="R7">
+      <c r="T7">
         <v>0</v>
       </c>
-      <c r="S7">
+      <c r="U7">
         <v>98.5</v>
       </c>
-      <c r="T7">
+      <c r="V7">
         <v>62.8</v>
       </c>
-      <c r="U7">
+      <c r="W7">
         <v>207.1</v>
       </c>
-      <c r="V7">
+      <c r="X7">
         <v>8.800000000000001</v>
       </c>
-      <c r="W7">
+      <c r="Y7">
         <v>28.6</v>
       </c>
-      <c r="X7">
+      <c r="Z7">
         <v>65</v>
       </c>
-      <c r="Y7">
+      <c r="AA7">
         <v>33</v>
       </c>
-      <c r="Z7">
+      <c r="AB7">
         <v>38</v>
       </c>
-      <c r="AA7">
+      <c r="AC7">
         <v>18</v>
       </c>
-      <c r="AB7">
+      <c r="AD7">
         <v>36</v>
       </c>
-      <c r="AC7">
+      <c r="AE7">
         <v>2</v>
       </c>
-      <c r="AD7">
+      <c r="AF7">
         <v>8</v>
       </c>
-      <c r="AE7">
+      <c r="AG7">
         <v>54</v>
       </c>
-      <c r="AF7">
+      <c r="AH7">
         <v>77.77777777777779</v>
       </c>
-      <c r="AG7">
+      <c r="AI7">
         <v>18.05555555555555</v>
       </c>
-      <c r="AH7">
+      <c r="AJ7">
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:34">
+    <row r="8" spans="1:36">
       <c r="A8" s="1">
         <v>251</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8">
+        <v>252</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8">
+        <v>36.28</v>
+      </c>
+      <c r="I8">
+        <v>22.93</v>
+      </c>
+      <c r="J8">
+        <v>33.24</v>
+      </c>
+      <c r="K8">
+        <v>7.55</v>
+      </c>
+      <c r="L8">
+        <v>97.59999999999999</v>
+      </c>
+      <c r="M8">
+        <v>68.7</v>
+      </c>
+      <c r="N8">
+        <v>1.55</v>
+      </c>
+      <c r="O8">
+        <v>2.04</v>
+      </c>
+      <c r="P8">
+        <v>80</v>
+      </c>
+      <c r="Q8">
+        <v>80</v>
+      </c>
+      <c r="R8">
+        <v>70</v>
+      </c>
+      <c r="S8">
+        <v>504</v>
+      </c>
+      <c r="T8">
+        <v>414</v>
+      </c>
+      <c r="U8">
+        <v>109.9</v>
+      </c>
+      <c r="V8">
+        <v>95.2</v>
+      </c>
+      <c r="W8">
+        <v>181.1</v>
+      </c>
+      <c r="X8">
+        <v>7.2</v>
+      </c>
+      <c r="Y8">
+        <v>32.1</v>
+      </c>
+      <c r="Z8">
+        <v>85</v>
+      </c>
+      <c r="AA8">
+        <v>53</v>
+      </c>
+      <c r="AB8">
+        <v>54</v>
+      </c>
+      <c r="AC8">
+        <v>40</v>
+      </c>
+      <c r="AD8">
+        <v>48</v>
+      </c>
+      <c r="AE8">
+        <v>6</v>
+      </c>
+      <c r="AF8">
+        <v>12</v>
+      </c>
+      <c r="AG8">
         <v>34</v>
       </c>
-      <c r="C8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8">
-        <v>36.28</v>
-      </c>
-      <c r="G8">
-        <v>22.93</v>
-      </c>
-      <c r="H8">
-        <v>33.24</v>
-      </c>
-      <c r="I8">
-        <v>7.55</v>
-      </c>
-      <c r="J8">
-        <v>97.59999999999999</v>
-      </c>
-      <c r="K8">
-        <v>68.7</v>
-      </c>
-      <c r="L8">
-        <v>1.55</v>
-      </c>
-      <c r="M8">
-        <v>2.04</v>
-      </c>
-      <c r="N8">
-        <v>80</v>
-      </c>
-      <c r="O8">
-        <v>80</v>
-      </c>
-      <c r="P8">
-        <v>70</v>
-      </c>
-      <c r="Q8">
-        <v>504</v>
-      </c>
-      <c r="R8">
-        <v>414</v>
-      </c>
-      <c r="S8">
-        <v>109.9</v>
-      </c>
-      <c r="T8">
-        <v>95.2</v>
-      </c>
-      <c r="U8">
-        <v>181.1</v>
-      </c>
-      <c r="V8">
-        <v>7.2</v>
-      </c>
-      <c r="W8">
-        <v>32.1</v>
-      </c>
-      <c r="X8">
-        <v>85</v>
-      </c>
-      <c r="Y8">
-        <v>53</v>
-      </c>
-      <c r="Z8">
-        <v>54</v>
-      </c>
-      <c r="AA8">
-        <v>40</v>
-      </c>
-      <c r="AB8">
-        <v>48</v>
-      </c>
-      <c r="AC8">
-        <v>6</v>
-      </c>
-      <c r="AD8">
-        <v>12</v>
-      </c>
-      <c r="AE8">
-        <v>34</v>
-      </c>
-      <c r="AF8">
+      <c r="AH8">
         <v>84.50704225352112</v>
       </c>
-      <c r="AG8">
+      <c r="AI8">
         <v>35.2112676056338</v>
       </c>
-      <c r="AH8">
+      <c r="AJ8">
         <v>152.5</v>
       </c>
     </row>
-    <row r="9" spans="1:34">
+    <row r="9" spans="1:36">
       <c r="A9" s="1">
         <v>282</v>
       </c>
-      <c r="B9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" t="s">
-        <v>39</v>
+      <c r="B9">
+        <v>283</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9">
+        <v>41</v>
+      </c>
+      <c r="F9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9">
         <v>16.55</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <v>22.3</v>
       </c>
-      <c r="H9">
+      <c r="J9">
         <v>36.9</v>
       </c>
-      <c r="I9">
+      <c r="K9">
         <v>24.25</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>98.09999999999999</v>
       </c>
-      <c r="K9">
+      <c r="M9">
         <v>71.90000000000001</v>
       </c>
-      <c r="L9">
+      <c r="N9">
         <v>0.24</v>
       </c>
-      <c r="M9">
+      <c r="O9">
         <v>2.76</v>
       </c>
-      <c r="N9">
+      <c r="P9">
         <v>80</v>
       </c>
-      <c r="O9">
+      <c r="Q9">
         <v>80</v>
       </c>
-      <c r="P9">
+      <c r="R9">
         <v>33.5</v>
       </c>
-      <c r="Q9">
+      <c r="S9">
         <v>241</v>
       </c>
-      <c r="R9">
+      <c r="T9">
         <v>151</v>
       </c>
-      <c r="S9">
+      <c r="U9">
         <v>127.7</v>
       </c>
-      <c r="T9">
+      <c r="V9">
         <v>118.2</v>
       </c>
-      <c r="U9">
+      <c r="W9">
         <v>199.4</v>
       </c>
-      <c r="V9">
+      <c r="X9">
         <v>6.7</v>
       </c>
-      <c r="W9">
+      <c r="Y9">
         <v>38.7</v>
       </c>
-      <c r="X9">
+      <c r="Z9">
         <v>91</v>
       </c>
-      <c r="Y9">
+      <c r="AA9">
         <v>60</v>
       </c>
-      <c r="Z9">
+      <c r="AB9">
         <v>63</v>
       </c>
-      <c r="AA9">
+      <c r="AC9">
         <v>59</v>
       </c>
-      <c r="AB9">
+      <c r="AD9">
         <v>61</v>
       </c>
-      <c r="AC9">
+      <c r="AE9">
         <v>2</v>
       </c>
-      <c r="AD9">
+      <c r="AF9">
         <v>11</v>
       </c>
-      <c r="AE9">
+      <c r="AG9">
         <v>26</v>
       </c>
-      <c r="AF9">
+      <c r="AH9">
         <v>63.01369863013699</v>
       </c>
-      <c r="AG9">
+      <c r="AI9">
         <v>5.47945205479452</v>
       </c>
     </row>
-    <row r="10" spans="1:34">
+    <row r="10" spans="1:36">
       <c r="A10" s="1">
         <v>287</v>
       </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" t="s">
-        <v>39</v>
+      <c r="B10">
+        <v>288</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10">
+        <v>41</v>
+      </c>
+      <c r="F10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10">
         <v>19.85</v>
       </c>
-      <c r="G10">
+      <c r="I10">
         <v>21.54</v>
       </c>
-      <c r="H10">
+      <c r="J10">
         <v>33.71</v>
       </c>
-      <c r="I10">
+      <c r="K10">
         <v>24.91</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>85</v>
       </c>
-      <c r="K10">
+      <c r="M10">
         <v>49.9</v>
       </c>
-      <c r="L10">
+      <c r="N10">
         <v>1.27</v>
       </c>
-      <c r="M10">
+      <c r="O10">
         <v>2.48</v>
       </c>
-      <c r="N10">
+      <c r="P10">
         <v>60</v>
       </c>
-      <c r="O10">
+      <c r="Q10">
         <v>75</v>
       </c>
-      <c r="P10">
+      <c r="R10">
         <v>28.5</v>
       </c>
-      <c r="Q10">
+      <c r="S10">
         <v>192</v>
-      </c>
-      <c r="R10">
-        <v>102</v>
-      </c>
-      <c r="S10">
-        <v>111</v>
       </c>
       <c r="T10">
         <v>102</v>
       </c>
       <c r="U10">
+        <v>111</v>
+      </c>
+      <c r="V10">
+        <v>102</v>
+      </c>
+      <c r="W10">
         <v>177.1</v>
       </c>
-      <c r="V10">
+      <c r="X10">
         <v>6.4</v>
       </c>
-      <c r="W10">
+      <c r="Y10">
         <v>37.1</v>
       </c>
-      <c r="X10">
+      <c r="Z10">
         <v>90</v>
       </c>
-      <c r="Y10">
+      <c r="AA10">
         <v>59</v>
       </c>
-      <c r="Z10">
+      <c r="AB10">
         <v>46</v>
       </c>
-      <c r="AA10">
+      <c r="AC10">
         <v>40</v>
       </c>
-      <c r="AB10">
+      <c r="AD10">
         <v>43</v>
       </c>
-      <c r="AC10">
+      <c r="AE10">
         <v>3</v>
       </c>
-      <c r="AD10">
+      <c r="AF10">
         <v>11</v>
       </c>
-      <c r="AE10">
+      <c r="AG10">
         <v>43</v>
       </c>
-      <c r="AF10">
+      <c r="AH10">
         <v>58.57142857142858</v>
       </c>
-      <c r="AG10">
+      <c r="AI10">
         <v>11.26760563380282</v>
       </c>
-      <c r="AH10">
+      <c r="AJ10">
         <v>141.6666666666667</v>
       </c>
     </row>
-    <row r="11" spans="1:34">
+    <row r="11" spans="1:36">
       <c r="A11" s="1">
         <v>49</v>
       </c>
       <c r="B11">
+        <v>50</v>
+      </c>
+      <c r="C11" s="2">
+        <v>42227</v>
+      </c>
+      <c r="D11">
         <v>165</v>
       </c>
-      <c r="C11">
+      <c r="E11">
         <v>30</v>
       </c>
-      <c r="D11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11">
+      <c r="F11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11">
         <v>30.29</v>
       </c>
-      <c r="G11">
+      <c r="I11">
         <v>5.16</v>
       </c>
-      <c r="H11">
+      <c r="J11">
         <v>40.45</v>
       </c>
-      <c r="I11">
+      <c r="K11">
         <v>24.1</v>
       </c>
-      <c r="J11">
+      <c r="L11">
         <v>84.5</v>
       </c>
-      <c r="K11">
+      <c r="M11">
         <v>56.8</v>
       </c>
-      <c r="L11">
+      <c r="N11">
         <v>77.5</v>
       </c>
-      <c r="M11">
+      <c r="O11">
         <v>0.62</v>
       </c>
-      <c r="N11">
+      <c r="P11">
         <v>50</v>
       </c>
-      <c r="O11">
+      <c r="Q11">
         <v>50</v>
       </c>
-      <c r="P11">
+      <c r="R11">
         <v>119</v>
       </c>
-      <c r="Q11">
+      <c r="S11">
         <v>535</v>
       </c>
-      <c r="R11">
+      <c r="T11">
         <v>445</v>
       </c>
-      <c r="S11">
+      <c r="U11">
         <v>82.7</v>
       </c>
-      <c r="T11">
+      <c r="V11">
         <v>65.59999999999999</v>
       </c>
-      <c r="U11">
+      <c r="W11">
         <v>165.9</v>
       </c>
-      <c r="V11">
+      <c r="X11">
         <v>7.5</v>
       </c>
-      <c r="W11">
+      <c r="Y11">
         <v>36.2</v>
       </c>
-      <c r="X11">
+      <c r="Z11">
         <v>77</v>
       </c>
-      <c r="Y11">
+      <c r="AA11">
         <v>40</v>
       </c>
-      <c r="Z11">
+      <c r="AB11">
         <v>70</v>
       </c>
-      <c r="AA11">
+      <c r="AC11">
         <v>45</v>
       </c>
-      <c r="AB11">
+      <c r="AD11">
         <v>58</v>
       </c>
-      <c r="AC11">
+      <c r="AE11">
         <v>12</v>
       </c>
-      <c r="AD11">
+      <c r="AF11">
         <v>12</v>
       </c>
-      <c r="AE11">
+      <c r="AG11">
         <v>18</v>
       </c>
-      <c r="AF11">
+      <c r="AH11">
         <v>71.60493827160494</v>
       </c>
-      <c r="AG11">
+      <c r="AI11">
         <v>23.07692307692308</v>
       </c>
-      <c r="AH11">
+      <c r="AJ11">
         <v>217.6666666666667</v>
       </c>
     </row>
-    <row r="12" spans="1:34">
+    <row r="12" spans="1:36">
       <c r="A12" s="1">
         <v>265</v>
       </c>
       <c r="B12">
+        <v>266</v>
+      </c>
+      <c r="C12" s="2">
+        <v>42227</v>
+      </c>
+      <c r="D12">
         <v>165</v>
       </c>
-      <c r="C12">
+      <c r="E12">
         <v>30</v>
       </c>
-      <c r="D12" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12">
+      <c r="F12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12">
         <v>30.29</v>
       </c>
-      <c r="G12">
+      <c r="I12">
         <v>5.16</v>
       </c>
-      <c r="H12">
+      <c r="J12">
         <v>40.45</v>
       </c>
-      <c r="I12">
+      <c r="K12">
         <v>24.1</v>
       </c>
-      <c r="J12">
+      <c r="L12">
         <v>84.5</v>
       </c>
-      <c r="K12">
+      <c r="M12">
         <v>56.8</v>
       </c>
-      <c r="L12">
+      <c r="N12">
         <v>77.5</v>
       </c>
-      <c r="M12">
+      <c r="O12">
         <v>0.62</v>
       </c>
-      <c r="N12">
+      <c r="P12">
         <v>50</v>
       </c>
-      <c r="O12">
+      <c r="Q12">
         <v>50</v>
       </c>
-      <c r="P12">
+      <c r="R12">
         <v>119</v>
       </c>
-      <c r="Q12">
+      <c r="S12">
         <v>535</v>
       </c>
-      <c r="R12">
+      <c r="T12">
         <v>445</v>
       </c>
-      <c r="S12">
+      <c r="U12">
         <v>82.7</v>
       </c>
-      <c r="T12">
+      <c r="V12">
         <v>65.59999999999999</v>
       </c>
-      <c r="U12">
+      <c r="W12">
         <v>165.9</v>
       </c>
-      <c r="V12">
+      <c r="X12">
         <v>7.5</v>
       </c>
-      <c r="W12">
+      <c r="Y12">
         <v>36.2</v>
       </c>
-      <c r="X12">
+      <c r="Z12">
         <v>77</v>
       </c>
-      <c r="Y12">
+      <c r="AA12">
         <v>40</v>
       </c>
-      <c r="Z12">
+      <c r="AB12">
         <v>70</v>
       </c>
-      <c r="AA12">
+      <c r="AC12">
         <v>45</v>
       </c>
-      <c r="AB12">
+      <c r="AD12">
         <v>58</v>
       </c>
-      <c r="AC12">
+      <c r="AE12">
         <v>12</v>
       </c>
-      <c r="AD12">
+      <c r="AF12">
         <v>12</v>
       </c>
-      <c r="AE12">
+      <c r="AG12">
         <v>18</v>
       </c>
-      <c r="AF12">
+      <c r="AH12">
         <v>71.60493827160494</v>
       </c>
-      <c r="AG12">
+      <c r="AI12">
         <v>23.07692307692308</v>
       </c>
-      <c r="AH12">
+      <c r="AJ12">
         <v>217.6666666666667</v>
       </c>
     </row>
-    <row r="13" spans="1:34">
+    <row r="13" spans="1:36">
       <c r="A13" s="1">
         <v>67</v>
       </c>
       <c r="B13">
+        <v>68</v>
+      </c>
+      <c r="C13" s="2">
+        <v>42227</v>
+      </c>
+      <c r="D13">
         <v>164</v>
       </c>
-      <c r="C13">
+      <c r="E13">
         <v>30</v>
       </c>
-      <c r="D13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13">
+      <c r="F13" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13">
         <v>22.96</v>
       </c>
-      <c r="G13">
+      <c r="I13">
         <v>38.16</v>
       </c>
-      <c r="H13">
+      <c r="J13">
         <v>28.75</v>
       </c>
-      <c r="I13">
+      <c r="K13">
         <v>10.13</v>
       </c>
-      <c r="J13">
+      <c r="L13">
         <v>80.40000000000001</v>
       </c>
-      <c r="K13">
+      <c r="M13">
         <v>46.1</v>
       </c>
-      <c r="L13">
+      <c r="N13">
         <v>56.8</v>
       </c>
-      <c r="M13">
+      <c r="O13">
         <v>3.94</v>
       </c>
-      <c r="N13">
+      <c r="P13">
         <v>40</v>
       </c>
-      <c r="O13">
+      <c r="Q13">
         <v>60</v>
       </c>
-      <c r="P13">
+      <c r="R13">
         <v>28.5</v>
       </c>
-      <c r="Q13">
+      <c r="S13">
         <v>153</v>
       </c>
-      <c r="R13">
+      <c r="T13">
         <v>63</v>
       </c>
-      <c r="S13">
+      <c r="U13">
         <v>76.5</v>
-      </c>
-      <c r="T13">
-        <v>59.1</v>
-      </c>
-      <c r="U13">
-        <v>155</v>
       </c>
       <c r="V13">
         <v>59.1</v>
       </c>
       <c r="W13">
+        <v>155</v>
+      </c>
+      <c r="X13">
+        <v>59.1</v>
+      </c>
+      <c r="Y13">
         <v>33</v>
       </c>
-      <c r="X13">
+      <c r="Z13">
         <v>78</v>
       </c>
-      <c r="Y13">
+      <c r="AA13">
         <v>44</v>
       </c>
-      <c r="Z13">
+      <c r="AB13">
         <v>62</v>
       </c>
-      <c r="AA13">
+      <c r="AC13">
         <v>26</v>
       </c>
-      <c r="AB13">
+      <c r="AD13">
         <v>39</v>
       </c>
-      <c r="AC13">
+      <c r="AE13">
         <v>23</v>
       </c>
-      <c r="AD13">
+      <c r="AF13">
         <v>19</v>
       </c>
-      <c r="AE13">
+      <c r="AG13">
         <v>19</v>
       </c>
-      <c r="AF13">
+      <c r="AH13">
         <v>70.88607594936708</v>
       </c>
-      <c r="AG13">
+      <c r="AI13">
         <v>10.12658227848101</v>
       </c>
     </row>
-    <row r="14" spans="1:34">
+    <row r="14" spans="1:36">
       <c r="A14" s="1">
         <v>288</v>
       </c>
       <c r="B14">
+        <v>289</v>
+      </c>
+      <c r="C14" s="2">
+        <v>42227</v>
+      </c>
+      <c r="D14">
         <v>164</v>
       </c>
-      <c r="C14">
+      <c r="E14">
         <v>30</v>
       </c>
-      <c r="D14" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F14">
+      <c r="F14" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14">
         <v>22.96</v>
       </c>
-      <c r="G14">
+      <c r="I14">
         <v>38.16</v>
       </c>
-      <c r="H14">
+      <c r="J14">
         <v>28.75</v>
       </c>
-      <c r="I14">
+      <c r="K14">
         <v>10.13</v>
       </c>
-      <c r="J14">
+      <c r="L14">
         <v>80.40000000000001</v>
       </c>
-      <c r="K14">
+      <c r="M14">
         <v>46.1</v>
       </c>
-      <c r="L14">
+      <c r="N14">
         <v>56.8</v>
       </c>
-      <c r="M14">
+      <c r="O14">
         <v>3.94</v>
       </c>
-      <c r="N14">
+      <c r="P14">
         <v>40</v>
       </c>
-      <c r="O14">
+      <c r="Q14">
         <v>60</v>
       </c>
-      <c r="P14">
+      <c r="R14">
         <v>28.5</v>
       </c>
-      <c r="Q14">
+      <c r="S14">
         <v>153</v>
       </c>
-      <c r="R14">
+      <c r="T14">
         <v>63</v>
       </c>
-      <c r="S14">
+      <c r="U14">
         <v>76.5</v>
-      </c>
-      <c r="T14">
-        <v>59.1</v>
-      </c>
-      <c r="U14">
-        <v>155</v>
       </c>
       <c r="V14">
         <v>59.1</v>
       </c>
       <c r="W14">
+        <v>155</v>
+      </c>
+      <c r="X14">
+        <v>59.1</v>
+      </c>
+      <c r="Y14">
         <v>33</v>
       </c>
-      <c r="X14">
+      <c r="Z14">
         <v>78</v>
       </c>
-      <c r="Y14">
+      <c r="AA14">
         <v>44</v>
       </c>
-      <c r="Z14">
+      <c r="AB14">
         <v>62</v>
       </c>
-      <c r="AA14">
+      <c r="AC14">
         <v>26</v>
       </c>
-      <c r="AB14">
+      <c r="AD14">
         <v>39</v>
       </c>
-      <c r="AC14">
+      <c r="AE14">
         <v>23</v>
       </c>
-      <c r="AD14">
+      <c r="AF14">
         <v>19</v>
       </c>
-      <c r="AE14">
+      <c r="AG14">
         <v>19</v>
       </c>
-      <c r="AF14">
+      <c r="AH14">
         <v>70.88607594936708</v>
       </c>
-      <c r="AG14">
+      <c r="AI14">
         <v>10.12658227848101</v>
       </c>
     </row>
-    <row r="15" spans="1:34">
+    <row r="15" spans="1:36">
       <c r="A15" s="1">
         <v>3</v>
       </c>
       <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15" s="2">
+        <v>42262</v>
+      </c>
+      <c r="D15">
         <v>205</v>
       </c>
-      <c r="C15">
+      <c r="E15">
         <v>36</v>
       </c>
-      <c r="D15" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15">
+      <c r="F15" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15">
         <v>130503</v>
       </c>
-      <c r="F15">
+      <c r="H15">
         <v>26.32</v>
       </c>
-      <c r="G15">
+      <c r="I15">
         <v>15.76</v>
       </c>
-      <c r="H15">
+      <c r="J15">
         <v>21.64</v>
       </c>
-      <c r="I15">
+      <c r="K15">
         <v>36.29</v>
       </c>
-      <c r="J15">
+      <c r="L15">
         <v>94.90000000000001</v>
       </c>
-      <c r="K15">
+      <c r="M15">
         <v>79.09999999999999</v>
       </c>
-      <c r="L15">
+      <c r="N15">
         <v>76.7</v>
       </c>
-      <c r="M15">
+      <c r="O15">
         <v>0.013</v>
       </c>
-      <c r="N15">
+      <c r="P15">
         <v>75</v>
       </c>
-      <c r="O15">
+      <c r="Q15">
         <v>75</v>
       </c>
-      <c r="P15">
+      <c r="R15">
         <v>57.5</v>
       </c>
-      <c r="Q15">
+      <c r="S15">
         <v>366</v>
       </c>
-      <c r="R15">
+      <c r="T15">
         <v>281</v>
       </c>
-      <c r="S15">
+      <c r="U15">
         <v>55.5</v>
       </c>
-      <c r="T15">
+      <c r="V15">
         <v>48.8</v>
       </c>
-      <c r="U15">
+      <c r="W15">
         <v>84.8</v>
       </c>
-      <c r="V15">
+      <c r="X15">
         <v>6.5</v>
       </c>
-      <c r="W15">
+      <c r="Y15">
         <v>29.9</v>
       </c>
-      <c r="X15">
+      <c r="Z15">
         <v>90</v>
       </c>
-      <c r="Y15">
+      <c r="AA15">
         <v>69</v>
       </c>
-      <c r="Z15">
+      <c r="AB15">
         <v>50</v>
       </c>
-      <c r="AA15">
+      <c r="AC15">
         <v>15</v>
       </c>
-      <c r="AB15">
+      <c r="AD15">
         <v>18</v>
       </c>
-      <c r="AC15">
+      <c r="AE15">
         <v>31</v>
       </c>
-      <c r="AD15">
+      <c r="AF15">
         <v>37</v>
       </c>
-      <c r="AE15">
+      <c r="AG15">
         <v>13</v>
       </c>
-      <c r="AF15">
+      <c r="AH15">
         <v>77.02702702702703</v>
       </c>
-      <c r="AG15">
+      <c r="AI15">
         <v>27.02702702702703</v>
       </c>
     </row>
-    <row r="16" spans="1:34">
+    <row r="16" spans="1:36">
       <c r="A16" s="1">
         <v>53</v>
       </c>
       <c r="B16">
+        <v>54</v>
+      </c>
+      <c r="C16" s="2">
+        <v>42262</v>
+      </c>
+      <c r="D16">
         <v>210</v>
       </c>
-      <c r="C16">
+      <c r="E16">
         <v>36</v>
       </c>
-      <c r="D16" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" t="s">
-        <v>56</v>
-      </c>
-      <c r="F16">
+      <c r="F16" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16">
         <v>27.65</v>
       </c>
-      <c r="G16">
+      <c r="I16">
         <v>29.35</v>
       </c>
-      <c r="H16">
+      <c r="J16">
         <v>32.08</v>
       </c>
-      <c r="I16">
+      <c r="K16">
         <v>10.92</v>
       </c>
-      <c r="J16">
+      <c r="L16">
         <v>95</v>
       </c>
-      <c r="K16">
+      <c r="M16">
         <v>83.59999999999999</v>
       </c>
-      <c r="L16">
+      <c r="N16">
         <v>79.40000000000001</v>
       </c>
-      <c r="M16">
+      <c r="O16">
         <v>0.013</v>
       </c>
-      <c r="N16">
+      <c r="P16">
         <v>65</v>
       </c>
-      <c r="O16">
+      <c r="Q16">
         <v>70</v>
       </c>
-      <c r="P16">
+      <c r="R16">
         <v>25</v>
       </c>
-      <c r="Q16">
+      <c r="S16">
         <v>148</v>
       </c>
-      <c r="R16">
+      <c r="T16">
         <v>63</v>
       </c>
-      <c r="S16">
+      <c r="U16">
         <v>81.2</v>
       </c>
-      <c r="T16">
+      <c r="V16">
         <v>68</v>
       </c>
-      <c r="U16">
+      <c r="W16">
         <v>142.5</v>
       </c>
-      <c r="V16">
+      <c r="X16">
         <v>6.9</v>
       </c>
-      <c r="W16">
+      <c r="Y16">
         <v>30.6</v>
       </c>
-      <c r="X16">
+      <c r="Z16">
         <v>84</v>
       </c>
-      <c r="Y16">
+      <c r="AA16">
         <v>57</v>
       </c>
-      <c r="Z16">
+      <c r="AB16">
         <v>57</v>
       </c>
-      <c r="AA16">
+      <c r="AC16">
         <v>29</v>
       </c>
-      <c r="AB16">
+      <c r="AD16">
         <v>38</v>
       </c>
-      <c r="AC16">
+      <c r="AE16">
         <v>19</v>
       </c>
-      <c r="AD16">
+      <c r="AF16">
         <v>24</v>
       </c>
-      <c r="AE16">
+      <c r="AG16">
         <v>18</v>
       </c>
-      <c r="AF16">
+      <c r="AH16">
         <v>60.56338028169014</v>
       </c>
-      <c r="AG16">
+      <c r="AI16">
         <v>5.555555555555555</v>
       </c>
-      <c r="AH16">
+      <c r="AJ16">
         <v>223.5</v>
       </c>
     </row>
-    <row r="17" spans="1:34">
+    <row r="17" spans="1:36">
       <c r="A17" s="1">
         <v>67</v>
       </c>
       <c r="B17">
+        <v>68</v>
+      </c>
+      <c r="C17" s="2">
+        <v>42227</v>
+      </c>
+      <c r="D17">
         <v>164</v>
       </c>
-      <c r="C17">
+      <c r="E17">
         <v>30</v>
       </c>
-      <c r="D17" t="s">
-        <v>45</v>
-      </c>
-      <c r="E17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F17">
+      <c r="F17" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" t="s">
+        <v>57</v>
+      </c>
+      <c r="H17">
         <v>22.96</v>
       </c>
-      <c r="G17">
+      <c r="I17">
         <v>38.16</v>
       </c>
-      <c r="H17">
+      <c r="J17">
         <v>28.75</v>
       </c>
-      <c r="I17">
+      <c r="K17">
         <v>10.13</v>
       </c>
-      <c r="J17">
+      <c r="L17">
         <v>80.40000000000001</v>
       </c>
-      <c r="K17">
+      <c r="M17">
         <v>46.1</v>
       </c>
-      <c r="L17">
+      <c r="N17">
         <v>56.8</v>
       </c>
-      <c r="M17">
+      <c r="O17">
         <v>3.94</v>
       </c>
-      <c r="N17">
+      <c r="P17">
         <v>40</v>
       </c>
-      <c r="O17">
+      <c r="Q17">
         <v>60</v>
       </c>
-      <c r="P17">
+      <c r="R17">
         <v>28.5</v>
       </c>
-      <c r="Q17">
+      <c r="S17">
         <v>153</v>
       </c>
-      <c r="R17">
+      <c r="T17">
         <v>63</v>
       </c>
-      <c r="S17">
+      <c r="U17">
         <v>76.5</v>
-      </c>
-      <c r="T17">
-        <v>59.1</v>
-      </c>
-      <c r="U17">
-        <v>155</v>
       </c>
       <c r="V17">
         <v>59.1</v>
       </c>
       <c r="W17">
+        <v>155</v>
+      </c>
+      <c r="X17">
+        <v>59.1</v>
+      </c>
+      <c r="Y17">
         <v>33</v>
       </c>
-      <c r="X17">
+      <c r="Z17">
         <v>78</v>
       </c>
-      <c r="Y17">
+      <c r="AA17">
         <v>44</v>
       </c>
-      <c r="Z17">
+      <c r="AB17">
         <v>62</v>
       </c>
-      <c r="AA17">
+      <c r="AC17">
         <v>26</v>
       </c>
-      <c r="AB17">
+      <c r="AD17">
         <v>39</v>
       </c>
-      <c r="AC17">
+      <c r="AE17">
         <v>23</v>
       </c>
-      <c r="AD17">
+      <c r="AF17">
         <v>19</v>
       </c>
-      <c r="AE17">
+      <c r="AG17">
         <v>19</v>
       </c>
-      <c r="AF17">
+      <c r="AH17">
         <v>70.88607594936708</v>
       </c>
-      <c r="AG17">
+      <c r="AI17">
         <v>10.12658227848101</v>
       </c>
     </row>
-    <row r="18" spans="1:34">
+    <row r="18" spans="1:36">
       <c r="A18" s="1">
         <v>177</v>
       </c>
-      <c r="B18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" t="s">
-        <v>38</v>
+      <c r="B18">
+        <v>178</v>
+      </c>
+      <c r="C18" s="2">
+        <v>43235</v>
       </c>
       <c r="D18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18">
+        <v>140513</v>
+      </c>
+      <c r="H18">
+        <v>33.04</v>
+      </c>
+      <c r="I18">
+        <v>25.28</v>
+      </c>
+      <c r="J18">
+        <v>30.16</v>
+      </c>
+      <c r="K18">
+        <v>11.53</v>
+      </c>
+      <c r="L18">
+        <v>89.5</v>
+      </c>
+      <c r="M18">
+        <v>99</v>
+      </c>
+      <c r="N18">
+        <v>71.7</v>
+      </c>
+      <c r="O18">
+        <v>0.17</v>
+      </c>
+      <c r="P18">
+        <v>60</v>
+      </c>
+      <c r="Q18">
+        <v>75</v>
+      </c>
+      <c r="R18">
+        <v>25</v>
+      </c>
+      <c r="S18">
+        <v>93.75</v>
+      </c>
+      <c r="T18">
+        <v>33.75</v>
+      </c>
+      <c r="U18">
+        <v>83.59999999999999</v>
+      </c>
+      <c r="V18">
+        <v>75.3</v>
+      </c>
+      <c r="W18">
+        <v>146</v>
+      </c>
+      <c r="X18">
+        <v>7.2</v>
+      </c>
+      <c r="Y18">
+        <v>32.6</v>
+      </c>
+      <c r="Z18">
+        <v>86</v>
+      </c>
+      <c r="AA18">
         <v>48</v>
       </c>
-      <c r="E18">
-        <v>140513</v>
-      </c>
-      <c r="F18">
-        <v>33.04</v>
-      </c>
-      <c r="G18">
-        <v>25.28</v>
-      </c>
-      <c r="H18">
-        <v>30.16</v>
-      </c>
-      <c r="I18">
-        <v>11.53</v>
-      </c>
-      <c r="J18">
-        <v>89.5</v>
-      </c>
-      <c r="K18">
-        <v>99</v>
-      </c>
-      <c r="L18">
-        <v>71.7</v>
-      </c>
-      <c r="M18">
-        <v>0.17</v>
-      </c>
-      <c r="N18">
+      <c r="AB18">
         <v>60</v>
       </c>
-      <c r="O18">
-        <v>75</v>
-      </c>
-      <c r="P18">
-        <v>25</v>
-      </c>
-      <c r="Q18">
-        <v>93.75</v>
-      </c>
-      <c r="R18">
-        <v>33.75</v>
-      </c>
-      <c r="S18">
-        <v>83.59999999999999</v>
-      </c>
-      <c r="T18">
-        <v>75.3</v>
-      </c>
-      <c r="U18">
-        <v>146</v>
-      </c>
-      <c r="V18">
-        <v>7.2</v>
-      </c>
-      <c r="W18">
-        <v>32.6</v>
-      </c>
-      <c r="X18">
-        <v>86</v>
-      </c>
-      <c r="Y18">
-        <v>48</v>
-      </c>
-      <c r="Z18">
-        <v>60</v>
-      </c>
-      <c r="AA18">
+      <c r="AC18">
         <v>33</v>
       </c>
-      <c r="AB18">
+      <c r="AD18">
         <v>36</v>
-      </c>
-      <c r="AC18">
-        <v>24</v>
-      </c>
-      <c r="AD18">
-        <v>16</v>
       </c>
       <c r="AE18">
         <v>24</v>
       </c>
       <c r="AF18">
+        <v>16</v>
+      </c>
+      <c r="AG18">
+        <v>24</v>
+      </c>
+      <c r="AH18">
         <v>72.58064516129032</v>
       </c>
-      <c r="AG18">
+      <c r="AI18">
         <v>17.74193548387097</v>
       </c>
     </row>
-    <row r="19" spans="1:34">
+    <row r="19" spans="1:36">
       <c r="A19" s="1">
         <v>187</v>
       </c>
       <c r="B19">
+        <v>188</v>
+      </c>
+      <c r="C19" s="2">
+        <v>42262</v>
+      </c>
+      <c r="D19">
         <v>205</v>
       </c>
-      <c r="C19">
+      <c r="E19">
         <v>36</v>
       </c>
-      <c r="D19" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19">
+      <c r="F19" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19">
         <v>130503</v>
       </c>
-      <c r="F19">
+      <c r="H19">
         <v>26.32</v>
       </c>
-      <c r="G19">
+      <c r="I19">
         <v>15.76</v>
       </c>
-      <c r="H19">
+      <c r="J19">
         <v>21.64</v>
       </c>
-      <c r="I19">
+      <c r="K19">
         <v>36.29</v>
       </c>
-      <c r="J19">
+      <c r="L19">
         <v>94.90000000000001</v>
       </c>
-      <c r="K19">
+      <c r="M19">
         <v>79.09999999999999</v>
       </c>
-      <c r="L19">
+      <c r="N19">
         <v>76.7</v>
       </c>
-      <c r="M19">
+      <c r="O19">
         <v>0.013</v>
       </c>
-      <c r="N19">
+      <c r="P19">
         <v>75</v>
       </c>
-      <c r="O19">
+      <c r="Q19">
         <v>75</v>
       </c>
-      <c r="P19">
+      <c r="R19">
         <v>57.5</v>
       </c>
-      <c r="Q19">
+      <c r="S19">
         <v>366</v>
       </c>
-      <c r="R19">
+      <c r="T19">
         <v>281</v>
       </c>
-      <c r="S19">
+      <c r="U19">
         <v>55.5</v>
       </c>
-      <c r="T19">
+      <c r="V19">
         <v>48.8</v>
       </c>
-      <c r="U19">
+      <c r="W19">
         <v>84.8</v>
       </c>
-      <c r="V19">
+      <c r="X19">
         <v>6.5</v>
       </c>
-      <c r="W19">
+      <c r="Y19">
         <v>29.9</v>
       </c>
-      <c r="X19">
+      <c r="Z19">
         <v>90</v>
       </c>
-      <c r="Y19">
+      <c r="AA19">
         <v>69</v>
       </c>
-      <c r="Z19">
+      <c r="AB19">
         <v>50</v>
       </c>
-      <c r="AA19">
+      <c r="AC19">
         <v>15</v>
       </c>
-      <c r="AB19">
+      <c r="AD19">
         <v>18</v>
       </c>
-      <c r="AC19">
+      <c r="AE19">
         <v>31</v>
       </c>
-      <c r="AD19">
+      <c r="AF19">
         <v>37</v>
       </c>
-      <c r="AE19">
+      <c r="AG19">
         <v>13</v>
       </c>
-      <c r="AF19">
+      <c r="AH19">
         <v>77.02702702702703</v>
       </c>
-      <c r="AG19">
+      <c r="AI19">
         <v>27.02702702702703</v>
       </c>
     </row>
-    <row r="20" spans="1:34">
+    <row r="20" spans="1:36">
       <c r="A20" s="1">
         <v>210</v>
       </c>
-      <c r="B20" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" t="s">
-        <v>38</v>
+      <c r="B20">
+        <v>211</v>
+      </c>
+      <c r="C20" s="2">
+        <v>43235</v>
       </c>
       <c r="D20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G20">
+        <v>140513</v>
+      </c>
+      <c r="H20">
+        <v>33.04</v>
+      </c>
+      <c r="I20">
+        <v>25.28</v>
+      </c>
+      <c r="J20">
+        <v>30.16</v>
+      </c>
+      <c r="K20">
+        <v>11.53</v>
+      </c>
+      <c r="L20">
+        <v>89.5</v>
+      </c>
+      <c r="M20">
+        <v>99</v>
+      </c>
+      <c r="N20">
+        <v>71.7</v>
+      </c>
+      <c r="O20">
+        <v>0.17</v>
+      </c>
+      <c r="P20">
+        <v>60</v>
+      </c>
+      <c r="Q20">
+        <v>75</v>
+      </c>
+      <c r="R20">
+        <v>25</v>
+      </c>
+      <c r="S20">
+        <v>93.75</v>
+      </c>
+      <c r="T20">
+        <v>33.75</v>
+      </c>
+      <c r="U20">
+        <v>83.59999999999999</v>
+      </c>
+      <c r="V20">
+        <v>75.3</v>
+      </c>
+      <c r="W20">
+        <v>146</v>
+      </c>
+      <c r="X20">
+        <v>7.2</v>
+      </c>
+      <c r="Y20">
+        <v>32.6</v>
+      </c>
+      <c r="Z20">
+        <v>86</v>
+      </c>
+      <c r="AA20">
         <v>48</v>
       </c>
-      <c r="E20">
-        <v>140513</v>
-      </c>
-      <c r="F20">
-        <v>33.04</v>
-      </c>
-      <c r="G20">
-        <v>25.28</v>
-      </c>
-      <c r="H20">
-        <v>30.16</v>
-      </c>
-      <c r="I20">
-        <v>11.53</v>
-      </c>
-      <c r="J20">
-        <v>89.5</v>
-      </c>
-      <c r="K20">
-        <v>99</v>
-      </c>
-      <c r="L20">
-        <v>71.7</v>
-      </c>
-      <c r="M20">
-        <v>0.17</v>
-      </c>
-      <c r="N20">
+      <c r="AB20">
         <v>60</v>
       </c>
-      <c r="O20">
-        <v>75</v>
-      </c>
-      <c r="P20">
-        <v>25</v>
-      </c>
-      <c r="Q20">
-        <v>93.75</v>
-      </c>
-      <c r="R20">
-        <v>33.75</v>
-      </c>
-      <c r="S20">
-        <v>83.59999999999999</v>
-      </c>
-      <c r="T20">
-        <v>75.3</v>
-      </c>
-      <c r="U20">
-        <v>146</v>
-      </c>
-      <c r="V20">
-        <v>7.2</v>
-      </c>
-      <c r="W20">
-        <v>32.6</v>
-      </c>
-      <c r="X20">
-        <v>86</v>
-      </c>
-      <c r="Y20">
-        <v>48</v>
-      </c>
-      <c r="Z20">
-        <v>60</v>
-      </c>
-      <c r="AA20">
+      <c r="AC20">
         <v>33</v>
       </c>
-      <c r="AB20">
+      <c r="AD20">
         <v>36</v>
-      </c>
-      <c r="AC20">
-        <v>24</v>
-      </c>
-      <c r="AD20">
-        <v>16</v>
       </c>
       <c r="AE20">
         <v>24</v>
       </c>
       <c r="AF20">
+        <v>16</v>
+      </c>
+      <c r="AG20">
+        <v>24</v>
+      </c>
+      <c r="AH20">
         <v>72.58064516129032</v>
       </c>
-      <c r="AG20">
+      <c r="AI20">
         <v>17.74193548387097</v>
       </c>
     </row>
-    <row r="21" spans="1:34">
+    <row r="21" spans="1:36">
       <c r="A21" s="1">
         <v>233</v>
       </c>
       <c r="B21">
+        <v>234</v>
+      </c>
+      <c r="C21" s="2">
+        <v>42262</v>
+      </c>
+      <c r="D21">
         <v>210</v>
       </c>
-      <c r="C21">
+      <c r="E21">
         <v>36</v>
       </c>
-      <c r="D21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E21" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21">
+      <c r="F21" t="s">
+        <v>49</v>
+      </c>
+      <c r="G21" t="s">
+        <v>58</v>
+      </c>
+      <c r="H21">
         <v>27.65</v>
       </c>
-      <c r="G21">
+      <c r="I21">
         <v>29.35</v>
       </c>
-      <c r="H21">
+      <c r="J21">
         <v>32.08</v>
       </c>
-      <c r="I21">
+      <c r="K21">
         <v>10.92</v>
       </c>
-      <c r="J21">
+      <c r="L21">
         <v>95</v>
       </c>
-      <c r="K21">
+      <c r="M21">
         <v>83.59999999999999</v>
       </c>
-      <c r="L21">
+      <c r="N21">
         <v>79.40000000000001</v>
       </c>
-      <c r="M21">
+      <c r="O21">
         <v>0.013</v>
       </c>
-      <c r="N21">
+      <c r="P21">
         <v>65</v>
       </c>
-      <c r="O21">
+      <c r="Q21">
         <v>70</v>
       </c>
-      <c r="P21">
+      <c r="R21">
         <v>25</v>
       </c>
-      <c r="Q21">
+      <c r="S21">
         <v>148</v>
       </c>
-      <c r="R21">
+      <c r="T21">
         <v>63</v>
       </c>
-      <c r="S21">
+      <c r="U21">
         <v>81.2</v>
       </c>
-      <c r="T21">
+      <c r="V21">
         <v>68</v>
       </c>
-      <c r="U21">
+      <c r="W21">
         <v>142.5</v>
       </c>
-      <c r="V21">
+      <c r="X21">
         <v>6.9</v>
       </c>
-      <c r="W21">
+      <c r="Y21">
         <v>30.6</v>
       </c>
-      <c r="X21">
+      <c r="Z21">
         <v>84</v>
       </c>
-      <c r="Y21">
+      <c r="AA21">
         <v>57</v>
       </c>
-      <c r="Z21">
+      <c r="AB21">
         <v>57</v>
       </c>
-      <c r="AA21">
+      <c r="AC21">
         <v>29</v>
       </c>
-      <c r="AB21">
+      <c r="AD21">
         <v>38</v>
       </c>
-      <c r="AC21">
+      <c r="AE21">
         <v>19</v>
       </c>
-      <c r="AD21">
+      <c r="AF21">
         <v>24</v>
       </c>
-      <c r="AE21">
+      <c r="AG21">
         <v>18</v>
       </c>
-      <c r="AF21">
+      <c r="AH21">
         <v>60.56338028169014</v>
       </c>
-      <c r="AG21">
+      <c r="AI21">
         <v>5.555555555555555</v>
       </c>
-      <c r="AH21">
+      <c r="AJ21">
         <v>223.5</v>
       </c>
     </row>
-    <row r="22" spans="1:34">
+    <row r="22" spans="1:36">
       <c r="A22" s="1">
         <v>288</v>
       </c>
       <c r="B22">
+        <v>289</v>
+      </c>
+      <c r="C22" s="2">
+        <v>42227</v>
+      </c>
+      <c r="D22">
         <v>164</v>
       </c>
-      <c r="C22">
+      <c r="E22">
         <v>30</v>
       </c>
-      <c r="D22" t="s">
-        <v>45</v>
-      </c>
-      <c r="E22" t="s">
-        <v>55</v>
-      </c>
-      <c r="F22">
+      <c r="F22" t="s">
+        <v>47</v>
+      </c>
+      <c r="G22" t="s">
+        <v>57</v>
+      </c>
+      <c r="H22">
         <v>22.96</v>
       </c>
-      <c r="G22">
+      <c r="I22">
         <v>38.16</v>
       </c>
-      <c r="H22">
+      <c r="J22">
         <v>28.75</v>
       </c>
-      <c r="I22">
+      <c r="K22">
         <v>10.13</v>
       </c>
-      <c r="J22">
+      <c r="L22">
         <v>80.40000000000001</v>
       </c>
-      <c r="K22">
+      <c r="M22">
         <v>46.1</v>
       </c>
-      <c r="L22">
+      <c r="N22">
         <v>56.8</v>
       </c>
-      <c r="M22">
+      <c r="O22">
         <v>3.94</v>
       </c>
-      <c r="N22">
+      <c r="P22">
         <v>40</v>
       </c>
-      <c r="O22">
+      <c r="Q22">
         <v>60</v>
       </c>
-      <c r="P22">
+      <c r="R22">
         <v>28.5</v>
       </c>
-      <c r="Q22">
+      <c r="S22">
         <v>153</v>
       </c>
-      <c r="R22">
+      <c r="T22">
         <v>63</v>
       </c>
-      <c r="S22">
+      <c r="U22">
         <v>76.5</v>
-      </c>
-      <c r="T22">
-        <v>59.1</v>
-      </c>
-      <c r="U22">
-        <v>155</v>
       </c>
       <c r="V22">
         <v>59.1</v>
       </c>
       <c r="W22">
+        <v>155</v>
+      </c>
+      <c r="X22">
+        <v>59.1</v>
+      </c>
+      <c r="Y22">
         <v>33</v>
       </c>
-      <c r="X22">
+      <c r="Z22">
         <v>78</v>
       </c>
-      <c r="Y22">
+      <c r="AA22">
         <v>44</v>
       </c>
-      <c r="Z22">
+      <c r="AB22">
         <v>62</v>
       </c>
-      <c r="AA22">
+      <c r="AC22">
         <v>26</v>
       </c>
-      <c r="AB22">
+      <c r="AD22">
         <v>39</v>
       </c>
-      <c r="AC22">
+      <c r="AE22">
         <v>23</v>
       </c>
-      <c r="AD22">
+      <c r="AF22">
         <v>19</v>
       </c>
-      <c r="AE22">
+      <c r="AG22">
         <v>19</v>
       </c>
-      <c r="AF22">
+      <c r="AH22">
         <v>70.88607594936708</v>
       </c>
-      <c r="AG22">
+      <c r="AI22">
         <v>10.12658227848101</v>
       </c>
     </row>

</xml_diff>